<commit_message>
Update report Dual Colors
</commit_message>
<xml_diff>
--- a/03. Engineering/036. Testing/Test Report/pLED_DualColors_TestReport_v1.0.xlsx
+++ b/03. Engineering/036. Testing/Test Report/pLED_DualColors_TestReport_v1.0.xlsx
@@ -310,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -338,25 +338,31 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -663,7 +669,7 @@
   <dimension ref="B1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,8 +912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,28 +1004,28 @@
       <c r="I4" s="4"/>
     </row>
     <row r="5" spans="2:9" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="14" t="s">
         <v>35</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="15">
         <v>41695</v>
       </c>
-      <c r="I5" s="10"/>
+      <c r="I5" s="12"/>
     </row>
     <row r="6" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
@@ -1046,54 +1052,54 @@
       <c r="I6" s="4"/>
     </row>
     <row r="7" spans="2:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="H7" s="17">
+      <c r="H7" s="19">
         <v>41695</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="I7" s="18" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="19">
         <v>41695</v>
       </c>
-      <c r="I8" s="14"/>
+      <c r="I8" s="16"/>
     </row>
     <row r="9" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
@@ -1154,7 +1160,7 @@
   <dimension ref="B1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1256,7 +1262,7 @@
       <c r="E5" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="11" t="s">
         <v>60</v>
       </c>
       <c r="G5" s="4" t="s">
@@ -1306,7 +1312,7 @@
       <c r="E7" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="11" t="s">
         <v>60</v>
       </c>
       <c r="G7" s="4" t="s">
@@ -1332,7 +1338,7 @@
       <c r="E8" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="11" t="s">
         <v>60</v>
       </c>
       <c r="G8" s="4" t="s">

</xml_diff>